<commit_message>
rubik b rotation solved
</commit_message>
<xml_diff>
--- a/Rubik/Moves.xlsx
+++ b/Rubik/Moves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierre/Development/19/CodingSchool19/Rubik/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4789B868-3258-4641-A38C-A7917EB9415C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D08A024-8357-9842-AD6B-F6E5CBA68AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="3600" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit" sheetId="3" r:id="rId1"/>
@@ -10016,7 +10016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD708263-05D2-7C4C-BFFD-02F351CC7042}">
   <dimension ref="A1:BD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -19341,7 +19341,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BD56"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="AD70" sqref="AD70"/>
     </sheetView>
   </sheetViews>
@@ -37989,8 +37989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BD56"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AB49" sqref="AB49"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38099,13 +38099,13 @@
         <v>0</v>
       </c>
       <c r="AH1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI1" s="1">
         <v>0</v>
       </c>
       <c r="AJ1" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK1" s="1">
         <v>0</v>
@@ -39107,13 +39107,13 @@
         <v>0</v>
       </c>
       <c r="AH7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="1">
         <v>0</v>
       </c>
       <c r="AJ7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7" s="1">
         <v>0</v>
@@ -47314,7 +47314,7 @@
   <dimension ref="A1:BD56"/>
   <sheetViews>
     <sheetView zoomScale="69" workbookViewId="0">
-      <selection activeCell="AB49" sqref="AB49"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>